<commit_message>
add yesterdays and todays task to progress report
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/CS340_S25_Leo/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C73DB3-D357-204E-9069-75FF51D41C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D752180D-D650-B143-A88C-29A9E2868098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Task Name</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>Everyone</t>
+  </si>
+  <si>
+    <t>Create github repo</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Adam Rodi</t>
+  </si>
+  <si>
+    <t>Decide on project idea</t>
+  </si>
+  <si>
+    <t>Design module communication diagram</t>
   </si>
 </sst>
 </file>
@@ -369,18 +384,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -405,9 +420,51 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45752</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add module design, and ppt slides for report
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/CS340_S25_Leo/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D752180D-D650-B143-A88C-29A9E2868098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA3BC65-B199-2443-B69E-EDAB1ABD130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Task Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Brainstorm project ideas</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Everyone</t>
   </si>
   <si>
@@ -61,6 +58,15 @@
   </si>
   <si>
     <t>Design module communication diagram</t>
+  </si>
+  <si>
+    <t>Complete PA1 powerpoint report</t>
+  </si>
+  <si>
+    <t>Design module outlines</t>
+  </si>
+  <si>
+    <t>Define input data format</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -420,10 +426,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -431,13 +437,13 @@
         <v>45752</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -445,13 +451,13 @@
         <v>45753</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -459,13 +465,55 @@
         <v>45753</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exporting YearlyAvgVolume to pickle file
proccess_data and visualize class now have global variables outputPath and inputPath to more easily export/read files from those directories. Can now export YearlyAvgVolume to pickle, and read from pickle.
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajsku\OneDrive\Documents\GitHub\CS340_S25_Leo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914901C6-1210-4958-8C19-F2390A6709AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EF661-229A-490B-A97E-7F3C6E6E90CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Task Name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Caleb Viverito</t>
+  </si>
+  <si>
+    <t>Added exporting Avg Volume Functions to pickle file</t>
   </si>
 </sst>
 </file>
@@ -399,21 +402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -427,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45751</v>
       </c>
@@ -441,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45752</v>
       </c>
@@ -455,7 +458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45753</v>
       </c>
@@ -469,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45753</v>
       </c>
@@ -483,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45753</v>
       </c>
@@ -497,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45753</v>
       </c>
@@ -511,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45753</v>
       </c>
@@ -525,7 +528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45761</v>
       </c>
@@ -536,6 +539,20 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>45762</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add exception handling to read/write functions
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajsku\OneDrive\Documents\GitHub\CS340_S25_Leo\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/CS340_S25_Leo/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EF661-229A-490B-A97E-7F3C6E6E90CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F62A29-04C3-3845-9713-A56A723FB033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Task Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Added exporting Avg Volume Functions to pickle file</t>
+  </si>
+  <si>
+    <t>Add exception handling to functions</t>
   </si>
 </sst>
 </file>
@@ -402,21 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -430,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45751</v>
       </c>
@@ -444,7 +447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45752</v>
       </c>
@@ -458,7 +461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45753</v>
       </c>
@@ -472,7 +475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45753</v>
       </c>
@@ -486,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45753</v>
       </c>
@@ -500,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45753</v>
       </c>
@@ -514,7 +517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45753</v>
       </c>
@@ -528,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45761</v>
       </c>
@@ -542,7 +545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45762</v>
       </c>
@@ -554,6 +557,20 @@
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>45765</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement price visualization functions
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/CS340_S25_Leo/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F62A29-04C3-3845-9713-A56A723FB033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C630B461-F4F4-D94C-B770-AD384DC540FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Task Name</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Add exception handling to functions</t>
+  </si>
+  <si>
+    <t>Implement price visualization functions</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -567,9 +570,23 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>45774</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added basic ui components
</commit_message>
<xml_diff>
--- a/Doc/TaskProgresReport.xlsx
+++ b/Doc/TaskProgresReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/CS340_S25_Leo/Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajsku\OneDrive\Documents\GitHub\CS340_S25_Leo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C630B461-F4F4-D94C-B770-AD384DC540FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E60ECF-8419-4457-A942-DC055A47A060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Task Name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Implement price visualization functions</t>
+  </si>
+  <si>
+    <t>Added basic console ui</t>
   </si>
 </sst>
 </file>
@@ -408,21 +411,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -436,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45751</v>
       </c>
@@ -450,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45752</v>
       </c>
@@ -464,7 +467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45753</v>
       </c>
@@ -478,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45753</v>
       </c>
@@ -492,7 +495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45753</v>
       </c>
@@ -506,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45753</v>
       </c>
@@ -520,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45753</v>
       </c>
@@ -534,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45761</v>
       </c>
@@ -542,13 +545,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45762</v>
       </c>
@@ -556,13 +559,13 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45765</v>
       </c>
@@ -576,7 +579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45774</v>
       </c>
@@ -588,6 +591,20 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45774</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>